<commit_message>
hours as of 13.09.23
</commit_message>
<xml_diff>
--- a/Hours/Attila/Attila hours.xlsx
+++ b/Hours/Attila/Attila hours.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulya\Documents\GitHub\MAMMAO\Hours\Attila\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gulya\Documents\Uni\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AE2A81-02A8-4EBB-81BC-7B09B193DD06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D300BF-E0BD-46AA-8197-757D11B1346E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -43,6 +43,36 @@
   </si>
   <si>
     <t>meeting</t>
+  </si>
+  <si>
+    <t>learning Arduino</t>
+  </si>
+  <si>
+    <t>07.09.2023</t>
+  </si>
+  <si>
+    <t>retroactively making the minutes</t>
+  </si>
+  <si>
+    <t>09.09.2023</t>
+  </si>
+  <si>
+    <t>getting to know the bt module, pt 1</t>
+  </si>
+  <si>
+    <t>12.09.2023</t>
+  </si>
+  <si>
+    <t>getting to know the bt module, pt 2</t>
+  </si>
+  <si>
+    <t>13.09.2023</t>
+  </si>
+  <si>
+    <t>meeting with tutor</t>
+  </si>
+  <si>
+    <t>making the Functional Design report</t>
   </si>
 </sst>
 </file>
@@ -84,9 +114,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -370,18 +406,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -394,7 +431,7 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -408,7 +445,7 @@
       <c r="C2" s="1">
         <v>0.44097222222222227</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -417,9 +454,120 @@
         <v>0.46875</v>
       </c>
       <c r="C3" s="1">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.53125</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.63194444444444442</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>